<commit_message>
Formula rewriting example for Java.
Requires v2.2.0
</commit_message>
<xml_diff>
--- a/Advanced/DoubleProcessing (.NET)/ResizeWithNesting.xlsx
+++ b/Advanced/DoubleProcessing (.NET)/ResizeWithNesting.xlsx
@@ -662,6 +662,54 @@
     <xf numFmtId="167" fontId="6" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -708,54 +756,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1107,17 +1107,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="62" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
       <c r="D1" s="1"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="49"/>
+      <c r="I1" s="49"/>
     </row>
     <row r="2" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
@@ -1138,8 +1138,8 @@
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
       <c r="G3" s="6"/>
-      <c r="H3" s="31"/>
-      <c r="I3" s="31"/>
+      <c r="H3" s="47"/>
+      <c r="I3" s="47"/>
     </row>
     <row r="4" spans="1:9" ht="2.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
@@ -1151,62 +1151,62 @@
       <c r="G4" s="3"/>
     </row>
     <row r="5" spans="1:9" ht="54.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="34" t="s">
+      <c r="A5" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="35"/>
-      <c r="C5" s="36"/>
+      <c r="B5" s="51"/>
+      <c r="C5" s="52"/>
       <c r="D5" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="43" t="s">
+      <c r="E5" s="59" t="s">
         <v>1</v>
       </c>
-      <c r="F5" s="43" t="s">
+      <c r="F5" s="59" t="s">
         <v>2</v>
       </c>
-      <c r="G5" s="43" t="s">
+      <c r="G5" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="H5" s="43" t="s">
+      <c r="H5" s="59" t="s">
         <v>24</v>
       </c>
-      <c r="I5" s="43" t="s">
+      <c r="I5" s="59" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="37"/>
-      <c r="B6" s="38"/>
-      <c r="C6" s="39"/>
+      <c r="A6" s="53"/>
+      <c r="B6" s="54"/>
+      <c r="C6" s="55"/>
       <c r="D6" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="44"/>
-      <c r="F6" s="44"/>
-      <c r="G6" s="44"/>
-      <c r="H6" s="44"/>
-      <c r="I6" s="44"/>
+      <c r="E6" s="60"/>
+      <c r="F6" s="60"/>
+      <c r="G6" s="60"/>
+      <c r="H6" s="60"/>
+      <c r="I6" s="60"/>
     </row>
     <row r="7" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="40"/>
-      <c r="B7" s="41"/>
-      <c r="C7" s="42"/>
+      <c r="A7" s="56"/>
+      <c r="B7" s="57"/>
+      <c r="C7" s="58"/>
       <c r="D7" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="45"/>
-      <c r="F7" s="45"/>
-      <c r="G7" s="45"/>
-      <c r="H7" s="45"/>
-      <c r="I7" s="45"/>
+      <c r="E7" s="61"/>
+      <c r="F7" s="61"/>
+      <c r="G7" s="61"/>
+      <c r="H7" s="61"/>
+      <c r="I7" s="61"/>
     </row>
     <row r="8" spans="1:9" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="47" t="s">
+      <c r="A8" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="48"/>
-      <c r="C8" s="49"/>
+      <c r="B8" s="32"/>
+      <c r="C8" s="33"/>
       <c r="D8" s="10" t="s">
         <v>21</v>
       </c>
@@ -1230,10 +1230,10 @@
       </c>
     </row>
     <row r="9" spans="1:9" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="61" t="s">
+      <c r="A9" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="62"/>
+      <c r="B9" s="46"/>
       <c r="C9" s="15" t="s">
         <v>16</v>
       </c>
@@ -1260,11 +1260,11 @@
       </c>
     </row>
     <row r="10" spans="1:9" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="47" t="s">
+      <c r="A10" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="48"/>
-      <c r="C10" s="49"/>
+      <c r="B10" s="32"/>
+      <c r="C10" s="33"/>
       <c r="D10" s="10" t="s">
         <v>23</v>
       </c>
@@ -1280,11 +1280,11 @@
       <c r="I10" s="14"/>
     </row>
     <row r="11" spans="1:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="50" t="s">
+      <c r="A11" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="51"/>
-      <c r="C11" s="52"/>
+      <c r="B11" s="35"/>
+      <c r="C11" s="36"/>
       <c r="D11" s="20">
         <f>SUM(D10:D10)</f>
         <v>0</v>
@@ -1302,11 +1302,11 @@
       <c r="I11" s="24"/>
     </row>
     <row r="12" spans="1:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="56" t="s">
+      <c r="A12" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="57"/>
-      <c r="C12" s="58"/>
+      <c r="B12" s="41"/>
+      <c r="C12" s="42"/>
       <c r="D12" s="25" t="e">
         <f>D11/E11</f>
         <v>#DIV/0!</v>
@@ -1318,23 +1318,23 @@
       <c r="I12" s="25"/>
     </row>
     <row r="13" spans="1:9" s="3" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="59"/>
-      <c r="B13" s="59"/>
-      <c r="C13" s="59"/>
-      <c r="D13" s="59"/>
+      <c r="A13" s="43"/>
+      <c r="B13" s="43"/>
+      <c r="C13" s="43"/>
+      <c r="D13" s="43"/>
     </row>
     <row r="14" spans="1:9" s="3" customFormat="1" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="60"/>
-      <c r="B14" s="60"/>
-      <c r="C14" s="60"/>
-      <c r="D14" s="60"/>
+      <c r="A14" s="44"/>
+      <c r="B14" s="44"/>
+      <c r="C14" s="44"/>
+      <c r="D14" s="44"/>
     </row>
     <row r="15" spans="1:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="53" t="s">
+      <c r="A15" s="37" t="s">
         <v>27</v>
       </c>
-      <c r="B15" s="54"/>
-      <c r="C15" s="55"/>
+      <c r="B15" s="38"/>
+      <c r="C15" s="39"/>
       <c r="D15" s="27" t="s">
         <v>12</v>
       </c>
@@ -1348,11 +1348,11 @@
       <c r="I15" s="30"/>
     </row>
     <row r="16" spans="1:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="53" t="s">
+      <c r="A16" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="B16" s="54"/>
-      <c r="C16" s="55"/>
+      <c r="B16" s="38"/>
+      <c r="C16" s="39"/>
       <c r="D16" s="27" t="s">
         <v>13</v>
       </c>
@@ -1366,11 +1366,11 @@
       <c r="I16" s="30"/>
     </row>
     <row r="17" spans="1:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="53" t="s">
+      <c r="A17" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="B17" s="54"/>
-      <c r="C17" s="55"/>
+      <c r="B17" s="38"/>
+      <c r="C17" s="39"/>
       <c r="D17" s="27" t="s">
         <v>18</v>
       </c>
@@ -1385,6 +1385,15 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="E1:I1"/>
+    <mergeCell ref="A5:C7"/>
+    <mergeCell ref="E5:E7"/>
+    <mergeCell ref="F5:F7"/>
+    <mergeCell ref="G5:G7"/>
+    <mergeCell ref="H5:H7"/>
+    <mergeCell ref="I5:I7"/>
+    <mergeCell ref="A1:C1"/>
     <mergeCell ref="A8:C8"/>
     <mergeCell ref="A11:C11"/>
     <mergeCell ref="A15:C15"/>
@@ -1394,15 +1403,6 @@
     <mergeCell ref="A10:C10"/>
     <mergeCell ref="A13:D14"/>
     <mergeCell ref="A9:B9"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="E1:I1"/>
-    <mergeCell ref="A5:C7"/>
-    <mergeCell ref="E5:E7"/>
-    <mergeCell ref="F5:F7"/>
-    <mergeCell ref="G5:G7"/>
-    <mergeCell ref="H5:H7"/>
-    <mergeCell ref="I5:I7"/>
-    <mergeCell ref="A1:C1"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0" right="0" top="0" bottom="0.5" header="0.5" footer="0.25"/>

</xml_diff>